<commit_message>
Ändrat solsken till minuter
</commit_message>
<xml_diff>
--- a/Data/Weather_data.xlsx
+++ b/Data/Weather_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbost\Documents\Nackademin\Programspråk\Gruppuppgift\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{21913133-6769-4680-BD83-68DDECDB12A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41301B3E-76F8-4374-B231-0CF2354965B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{57409BA4-BC29-4966-ACDA-D8D81C35AE8E}"/>
   </bookViews>
@@ -35,9 +35,6 @@
     <t>Station</t>
   </si>
   <si>
-    <t>Solskenssekunder_avg</t>
-  </si>
-  <si>
     <t>Temepratur_avg</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Kiruna</t>
+  </si>
+  <si>
+    <t>Solskensminuter_avg</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,21 +466,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>1477.6</v>
+        <v>25</v>
       </c>
       <c r="C2">
         <v>13.3</v>
@@ -491,10 +491,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>1399.1</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>13.8</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>1353.8</v>
+        <v>23</v>
       </c>
       <c r="C4">
         <v>15.2</v>
@@ -519,10 +519,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>1552</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>14.6</v>
@@ -533,10 +533,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>1497.1</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>14.5</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>1469.9</v>
+        <v>24</v>
       </c>
       <c r="C7">
         <v>10.5</v>
@@ -561,10 +561,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>1066.8</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>7.8</v>
@@ -575,10 +575,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>1789.8</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <v>14.7</v>
@@ -589,24 +589,24 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>1325.6</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
-        <v>1468.8</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>11</v>
@@ -617,24 +617,24 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>1487.2</v>
+        <v>25</v>
       </c>
       <c r="C12">
         <v>15.4</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13">
-        <v>1770.2</v>
+        <v>30</v>
       </c>
       <c r="C13">
         <v>14.1</v>
@@ -645,10 +645,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14">
-        <v>1674.5</v>
+        <v>28</v>
       </c>
       <c r="C14">
         <v>13.9</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>1844.3</v>
+        <v>31</v>
       </c>
       <c r="C15">
         <v>13.7</v>
@@ -673,10 +673,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>1372.3</v>
+        <v>23</v>
       </c>
       <c r="C16">
         <v>12.6</v>
@@ -687,10 +687,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>1787.2</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>11.2</v>
@@ -701,10 +701,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18">
-        <v>1779.5</v>
+        <v>30</v>
       </c>
       <c r="C18">
         <v>13.6</v>
@@ -715,13 +715,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19">
-        <v>960.6</v>
+        <v>16</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>3.9</v>
@@ -729,10 +729,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>1136.0999999999999</v>
+        <v>19</v>
       </c>
       <c r="C20">
         <v>7.8</v>

</xml_diff>